<commit_message>
add stats for SIFT vs YOLO
</commit_message>
<xml_diff>
--- a/saved_weights/SIFTandTracker_vs_YOLO_Scenario/stats.xlsx
+++ b/saved_weights/SIFTandTracker_vs_YOLO_Scenario/stats.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kuliah\Tugas Akhir\05111540000055_PBaskara\src\saved_weights\SIFTandTracker_vs_YOLO_Scenario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dip_Official\src\Tugas-Akhir\saved_weights\SIFTandTracker_vs_YOLO_Scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
-  <si>
-    <t>Deteksi</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Aktual</t>
   </si>
@@ -36,6 +33,12 @@
   </si>
   <si>
     <t>All Accuracy</t>
+  </si>
+  <si>
+    <t>SIFT Det</t>
+  </si>
+  <si>
+    <t>YOLO Det</t>
   </si>
 </sst>
 </file>
@@ -353,29 +356,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>95</v>
       </c>
@@ -385,6 +394,9 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>161</v>
       </c>
@@ -394,8 +406,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>96</v>
       </c>
@@ -405,6 +420,9 @@
       <c r="C3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <v>162</v>
       </c>
@@ -414,8 +432,11 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>97</v>
       </c>
@@ -425,6 +446,9 @@
       <c r="C4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <v>163</v>
       </c>
@@ -434,8 +458,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>98</v>
       </c>
@@ -445,6 +472,9 @@
       <c r="C5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5">
         <v>164</v>
       </c>
@@ -454,8 +484,11 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>99</v>
       </c>
@@ -465,6 +498,9 @@
       <c r="C6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
         <v>165</v>
       </c>
@@ -474,8 +510,11 @@
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>100</v>
       </c>
@@ -485,6 +524,9 @@
       <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="E7">
         <v>166</v>
       </c>
@@ -494,8 +536,11 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>101</v>
       </c>
@@ -505,6 +550,9 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8">
         <v>167</v>
       </c>
@@ -514,8 +562,11 @@
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>102</v>
       </c>
@@ -525,6 +576,9 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <v>168</v>
       </c>
@@ -534,8 +588,11 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>103</v>
       </c>
@@ -545,6 +602,9 @@
       <c r="C10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="E10">
         <v>169</v>
       </c>
@@ -554,8 +614,11 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>104</v>
       </c>
@@ -565,6 +628,9 @@
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="E11">
         <v>170</v>
       </c>
@@ -574,8 +640,11 @@
       <c r="G11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>105</v>
       </c>
@@ -585,6 +654,9 @@
       <c r="C12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <v>171</v>
       </c>
@@ -594,8 +666,11 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>106</v>
       </c>
@@ -605,6 +680,9 @@
       <c r="C13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <v>172</v>
       </c>
@@ -614,8 +692,11 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>107</v>
       </c>
@@ -625,6 +706,9 @@
       <c r="C14">
         <v>0</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <v>173</v>
       </c>
@@ -634,8 +718,11 @@
       <c r="G14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>108</v>
       </c>
@@ -645,6 +732,9 @@
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="E15">
         <v>174</v>
       </c>
@@ -654,8 +744,11 @@
       <c r="G15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>109</v>
       </c>
@@ -665,6 +758,9 @@
       <c r="C16">
         <v>0</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="E16">
         <v>175</v>
       </c>
@@ -674,8 +770,11 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>110</v>
       </c>
@@ -685,6 +784,9 @@
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="E17">
         <v>176</v>
       </c>
@@ -694,8 +796,11 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>111</v>
       </c>
@@ -705,6 +810,9 @@
       <c r="C18">
         <v>0</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="E18">
         <v>177</v>
       </c>
@@ -714,8 +822,11 @@
       <c r="G18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>112</v>
       </c>
@@ -725,6 +836,9 @@
       <c r="C19">
         <v>0</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="E19">
         <v>715</v>
       </c>
@@ -734,8 +848,11 @@
       <c r="G19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>113</v>
       </c>
@@ -745,6 +862,9 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
       <c r="E20">
         <v>716</v>
       </c>
@@ -754,8 +874,11 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>114</v>
       </c>
@@ -765,6 +888,9 @@
       <c r="C21">
         <v>1</v>
       </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
       <c r="E21">
         <v>717</v>
       </c>
@@ -774,8 +900,11 @@
       <c r="G21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>115</v>
       </c>
@@ -785,6 +914,9 @@
       <c r="C22">
         <v>1</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
       <c r="E22">
         <v>718</v>
       </c>
@@ -794,8 +926,11 @@
       <c r="G22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>116</v>
       </c>
@@ -805,6 +940,9 @@
       <c r="C23">
         <v>1</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="E23">
         <v>719</v>
       </c>
@@ -814,8 +952,11 @@
       <c r="G23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>117</v>
       </c>
@@ -825,6 +966,9 @@
       <c r="C24">
         <v>1</v>
       </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
       <c r="E24">
         <v>720</v>
       </c>
@@ -834,8 +978,11 @@
       <c r="G24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>118</v>
       </c>
@@ -845,6 +992,9 @@
       <c r="C25">
         <v>1</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="E25">
         <v>721</v>
       </c>
@@ -854,8 +1004,11 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>119</v>
       </c>
@@ -865,6 +1018,9 @@
       <c r="C26">
         <v>1</v>
       </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="E26">
         <v>722</v>
       </c>
@@ -874,8 +1030,11 @@
       <c r="G26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>120</v>
       </c>
@@ -885,6 +1044,9 @@
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
       <c r="E27">
         <v>723</v>
       </c>
@@ -894,8 +1056,11 @@
       <c r="G27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>121</v>
       </c>
@@ -905,6 +1070,9 @@
       <c r="C28">
         <v>1</v>
       </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
       <c r="E28">
         <v>724</v>
       </c>
@@ -914,8 +1082,11 @@
       <c r="G28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>122</v>
       </c>
@@ -925,6 +1096,9 @@
       <c r="C29">
         <v>1</v>
       </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
       <c r="E29">
         <v>725</v>
       </c>
@@ -934,8 +1108,11 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>123</v>
       </c>
@@ -945,6 +1122,9 @@
       <c r="C30">
         <v>1</v>
       </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
       <c r="E30">
         <v>726</v>
       </c>
@@ -954,8 +1134,11 @@
       <c r="G30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>324</v>
       </c>
@@ -965,6 +1148,9 @@
       <c r="C31">
         <v>0</v>
       </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
       <c r="E31">
         <v>727</v>
       </c>
@@ -974,8 +1160,11 @@
       <c r="G31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>325</v>
       </c>
@@ -985,6 +1174,9 @@
       <c r="C32">
         <v>0</v>
       </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
       <c r="E32">
         <v>728</v>
       </c>
@@ -994,8 +1186,11 @@
       <c r="G32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>326</v>
       </c>
@@ -1005,6 +1200,9 @@
       <c r="C33">
         <v>0</v>
       </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
       <c r="E33">
         <v>729</v>
       </c>
@@ -1014,8 +1212,11 @@
       <c r="G33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>327</v>
       </c>
@@ -1025,6 +1226,9 @@
       <c r="C34">
         <v>0</v>
       </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
       <c r="E34">
         <v>730</v>
       </c>
@@ -1034,8 +1238,11 @@
       <c r="G34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>328</v>
       </c>
@@ -1045,6 +1252,9 @@
       <c r="C35">
         <v>0</v>
       </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
       <c r="E35">
         <v>731</v>
       </c>
@@ -1054,8 +1264,11 @@
       <c r="G35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>329</v>
       </c>
@@ -1065,6 +1278,9 @@
       <c r="C36">
         <v>0</v>
       </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
       <c r="E36">
         <v>732</v>
       </c>
@@ -1074,8 +1290,11 @@
       <c r="G36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>330</v>
       </c>
@@ -1085,6 +1304,9 @@
       <c r="C37">
         <v>0</v>
       </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
       <c r="E37">
         <v>733</v>
       </c>
@@ -1094,8 +1316,11 @@
       <c r="G37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>331</v>
       </c>
@@ -1105,6 +1330,9 @@
       <c r="C38">
         <v>0</v>
       </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
       <c r="E38">
         <v>1066</v>
       </c>
@@ -1114,8 +1342,11 @@
       <c r="G38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>332</v>
       </c>
@@ -1125,6 +1356,9 @@
       <c r="C39">
         <v>0</v>
       </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
       <c r="E39">
         <v>1067</v>
       </c>
@@ -1134,8 +1368,11 @@
       <c r="G39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>333</v>
       </c>
@@ -1145,6 +1382,9 @@
       <c r="C40">
         <v>0</v>
       </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
       <c r="E40">
         <v>1068</v>
       </c>
@@ -1154,8 +1394,11 @@
       <c r="G40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>334</v>
       </c>
@@ -1165,6 +1408,9 @@
       <c r="C41">
         <v>0</v>
       </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
       <c r="E41">
         <v>1069</v>
       </c>
@@ -1174,8 +1420,11 @@
       <c r="G41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>335</v>
       </c>
@@ -1185,6 +1434,9 @@
       <c r="C42">
         <v>0</v>
       </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
       <c r="E42">
         <v>1070</v>
       </c>
@@ -1194,8 +1446,11 @@
       <c r="G42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>336</v>
       </c>
@@ -1205,6 +1460,9 @@
       <c r="C43">
         <v>0</v>
       </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
       <c r="E43">
         <v>1071</v>
       </c>
@@ -1214,8 +1472,11 @@
       <c r="G43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>337</v>
       </c>
@@ -1225,6 +1486,9 @@
       <c r="C44">
         <v>0</v>
       </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
       <c r="E44">
         <v>1072</v>
       </c>
@@ -1234,8 +1498,11 @@
       <c r="G44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>338</v>
       </c>
@@ -1245,6 +1512,9 @@
       <c r="C45">
         <v>0</v>
       </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
       <c r="E45">
         <v>1073</v>
       </c>
@@ -1254,8 +1524,11 @@
       <c r="G45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>339</v>
       </c>
@@ -1265,6 +1538,9 @@
       <c r="C46">
         <v>1</v>
       </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
       <c r="E46">
         <v>1074</v>
       </c>
@@ -1274,8 +1550,11 @@
       <c r="G46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>340</v>
       </c>
@@ -1285,6 +1564,9 @@
       <c r="C47">
         <v>1</v>
       </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
       <c r="E47">
         <v>1075</v>
       </c>
@@ -1294,8 +1576,11 @@
       <c r="G47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>341</v>
       </c>
@@ -1305,6 +1590,9 @@
       <c r="C48">
         <v>1</v>
       </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
       <c r="E48">
         <v>1076</v>
       </c>
@@ -1314,8 +1602,11 @@
       <c r="G48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>342</v>
       </c>
@@ -1325,6 +1616,9 @@
       <c r="C49">
         <v>1</v>
       </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
       <c r="E49">
         <v>1077</v>
       </c>
@@ -1334,8 +1628,11 @@
       <c r="G49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>343</v>
       </c>
@@ -1345,6 +1642,9 @@
       <c r="C50">
         <v>1</v>
       </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
       <c r="E50">
         <v>1078</v>
       </c>
@@ -1354,8 +1654,11 @@
       <c r="G50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>344</v>
       </c>
@@ -1365,6 +1668,9 @@
       <c r="C51">
         <v>1</v>
       </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
       <c r="E51">
         <v>1079</v>
       </c>
@@ -1374,8 +1680,11 @@
       <c r="G51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>345</v>
       </c>
@@ -1385,6 +1694,9 @@
       <c r="C52">
         <v>1</v>
       </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
       <c r="E52">
         <v>1080</v>
       </c>
@@ -1394,8 +1706,11 @@
       <c r="G52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>346</v>
       </c>
@@ -1405,6 +1720,9 @@
       <c r="C53">
         <v>1</v>
       </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
       <c r="E53">
         <v>1081</v>
       </c>
@@ -1414,8 +1732,11 @@
       <c r="G53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>347</v>
       </c>
@@ -1425,6 +1746,9 @@
       <c r="C54">
         <v>1</v>
       </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
       <c r="E54">
         <v>1082</v>
       </c>
@@ -1434,8 +1758,11 @@
       <c r="G54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>348</v>
       </c>
@@ -1443,6 +1770,9 @@
         <v>1</v>
       </c>
       <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
         <v>1</v>
       </c>
       <c r="F55">
@@ -1453,8 +1783,12 @@
         <f>SUM(G2:G54)</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <f>SUM(H2:H54)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>349</v>
       </c>
@@ -1464,15 +1798,22 @@
       <c r="C56">
         <v>1</v>
       </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
       <c r="E56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <f>(G55/F55*100)</f>
         <v>43.39622641509434</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <f>(H55/F55*100)</f>
+        <v>69.811320754716974</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>350</v>
       </c>
@@ -1482,8 +1823,11 @@
       <c r="C57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>351</v>
       </c>
@@ -1493,8 +1837,11 @@
       <c r="C58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>452</v>
       </c>
@@ -1504,8 +1851,11 @@
       <c r="C59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>453</v>
       </c>
@@ -1515,8 +1865,11 @@
       <c r="C60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>454</v>
       </c>
@@ -1526,8 +1879,11 @@
       <c r="C61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>455</v>
       </c>
@@ -1537,8 +1893,11 @@
       <c r="C62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>456</v>
       </c>
@@ -1548,8 +1907,11 @@
       <c r="C63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>457</v>
       </c>
@@ -1559,8 +1921,11 @@
       <c r="C64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>458</v>
       </c>
@@ -1570,8 +1935,11 @@
       <c r="C65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>459</v>
       </c>
@@ -1581,8 +1949,11 @@
       <c r="C66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>460</v>
       </c>
@@ -1592,8 +1963,11 @@
       <c r="C67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>461</v>
       </c>
@@ -1603,8 +1977,11 @@
       <c r="C68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>462</v>
       </c>
@@ -1614,8 +1991,11 @@
       <c r="C69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>463</v>
       </c>
@@ -1625,8 +2005,11 @@
       <c r="C70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>464</v>
       </c>
@@ -1636,8 +2019,11 @@
       <c r="C71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>465</v>
       </c>
@@ -1647,8 +2033,11 @@
       <c r="C72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>466</v>
       </c>
@@ -1658,8 +2047,11 @@
       <c r="C73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>467</v>
       </c>
@@ -1669,8 +2061,11 @@
       <c r="C74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>468</v>
       </c>
@@ -1680,8 +2075,11 @@
       <c r="C75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>469</v>
       </c>
@@ -1691,8 +2089,11 @@
       <c r="C76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>470</v>
       </c>
@@ -1702,8 +2103,11 @@
       <c r="C77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>471</v>
       </c>
@@ -1713,8 +2117,11 @@
       <c r="C78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>472</v>
       </c>
@@ -1724,8 +2131,11 @@
       <c r="C79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>473</v>
       </c>
@@ -1735,8 +2145,11 @@
       <c r="C80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>474</v>
       </c>
@@ -1746,8 +2159,11 @@
       <c r="C81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>475</v>
       </c>
@@ -1757,8 +2173,11 @@
       <c r="C82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>476</v>
       </c>
@@ -1768,8 +2187,11 @@
       <c r="C83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>477</v>
       </c>
@@ -1779,8 +2201,11 @@
       <c r="C84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>478</v>
       </c>
@@ -1790,8 +2215,11 @@
       <c r="C85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>479</v>
       </c>
@@ -1801,8 +2229,11 @@
       <c r="C86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>480</v>
       </c>
@@ -1812,8 +2243,11 @@
       <c r="C87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>481</v>
       </c>
@@ -1823,8 +2257,11 @@
       <c r="C88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>482</v>
       </c>
@@ -1834,8 +2271,11 @@
       <c r="C89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>483</v>
       </c>
@@ -1845,8 +2285,11 @@
       <c r="C90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>484</v>
       </c>
@@ -1856,8 +2299,11 @@
       <c r="C91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>485</v>
       </c>
@@ -1867,8 +2313,11 @@
       <c r="C92">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>486</v>
       </c>
@@ -1878,8 +2327,11 @@
       <c r="C93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>575</v>
       </c>
@@ -1889,8 +2341,11 @@
       <c r="C94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>576</v>
       </c>
@@ -1900,8 +2355,11 @@
       <c r="C95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>577</v>
       </c>
@@ -1911,8 +2369,11 @@
       <c r="C96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>578</v>
       </c>
@@ -1922,8 +2383,11 @@
       <c r="C97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>579</v>
       </c>
@@ -1933,8 +2397,11 @@
       <c r="C98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>580</v>
       </c>
@@ -1944,8 +2411,11 @@
       <c r="C99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>581</v>
       </c>
@@ -1955,8 +2425,11 @@
       <c r="C100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>582</v>
       </c>
@@ -1966,8 +2439,11 @@
       <c r="C101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>583</v>
       </c>
@@ -1977,8 +2453,11 @@
       <c r="C102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>584</v>
       </c>
@@ -1988,8 +2467,11 @@
       <c r="C103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>585</v>
       </c>
@@ -1999,8 +2481,11 @@
       <c r="C104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>586</v>
       </c>
@@ -2010,8 +2495,11 @@
       <c r="C105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>587</v>
       </c>
@@ -2021,8 +2509,11 @@
       <c r="C106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>588</v>
       </c>
@@ -2032,8 +2523,11 @@
       <c r="C107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>589</v>
       </c>
@@ -2043,8 +2537,11 @@
       <c r="C108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>590</v>
       </c>
@@ -2054,8 +2551,11 @@
       <c r="C109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>591</v>
       </c>
@@ -2065,8 +2565,11 @@
       <c r="C110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>592</v>
       </c>
@@ -2076,8 +2579,11 @@
       <c r="C111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>593</v>
       </c>
@@ -2087,8 +2593,11 @@
       <c r="C112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>594</v>
       </c>
@@ -2098,8 +2607,11 @@
       <c r="C113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>595</v>
       </c>
@@ -2109,8 +2621,11 @@
       <c r="C114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>596</v>
       </c>
@@ -2120,8 +2635,11 @@
       <c r="C115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>597</v>
       </c>
@@ -2131,8 +2649,11 @@
       <c r="C116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>598</v>
       </c>
@@ -2142,8 +2663,11 @@
       <c r="C117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>599</v>
       </c>
@@ -2153,8 +2677,11 @@
       <c r="C118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>600</v>
       </c>
@@ -2164,8 +2691,11 @@
       <c r="C119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>601</v>
       </c>
@@ -2175,8 +2705,11 @@
       <c r="C120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>634</v>
       </c>
@@ -2186,8 +2719,11 @@
       <c r="C121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>635</v>
       </c>
@@ -2197,8 +2733,11 @@
       <c r="C122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>636</v>
       </c>
@@ -2208,8 +2747,11 @@
       <c r="C123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>637</v>
       </c>
@@ -2219,8 +2761,11 @@
       <c r="C124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>638</v>
       </c>
@@ -2230,8 +2775,11 @@
       <c r="C125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>639</v>
       </c>
@@ -2241,8 +2789,11 @@
       <c r="C126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>640</v>
       </c>
@@ -2252,8 +2803,11 @@
       <c r="C127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>641</v>
       </c>
@@ -2263,8 +2817,11 @@
       <c r="C128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>642</v>
       </c>
@@ -2274,8 +2831,11 @@
       <c r="C129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>643</v>
       </c>
@@ -2285,8 +2845,11 @@
       <c r="C130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>644</v>
       </c>
@@ -2296,8 +2859,11 @@
       <c r="C131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>645</v>
       </c>
@@ -2307,8 +2873,11 @@
       <c r="C132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>646</v>
       </c>
@@ -2318,8 +2887,11 @@
       <c r="C133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>647</v>
       </c>
@@ -2329,8 +2901,11 @@
       <c r="C134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>648</v>
       </c>
@@ -2340,8 +2915,11 @@
       <c r="C135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>649</v>
       </c>
@@ -2351,8 +2929,11 @@
       <c r="C136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>650</v>
       </c>
@@ -2362,8 +2943,11 @@
       <c r="C137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B138">
         <f>SUM(B2:B137)</f>
         <v>136</v>
@@ -2372,21 +2956,33 @@
         <f>SUM(C2:C137)</f>
         <v>56</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <f>SUM(D2:D137)</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C139">
         <f>(C138/B138*100)</f>
         <v>41.17647058823529</v>
       </c>
+      <c r="D139">
+        <f>(D138/B138*100)</f>
+        <v>97.058823529411768</v>
+      </c>
       <c r="F139" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G139">
         <f>((C138+G55)/(B138+F55)*100)</f>
         <v>41.798941798941797</v>
+      </c>
+      <c r="H139">
+        <f>((H55+D138)/(B138+F55)*100)</f>
+        <v>89.417989417989418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update SIFTvsYOLO result statistic
</commit_message>
<xml_diff>
--- a/saved_weights/SIFTandTracker_vs_YOLO_Scenario/stats.xlsx
+++ b/saved_weights/SIFTandTracker_vs_YOLO_Scenario/stats.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dip_Official\src\Tugas-Akhir\saved_weights\SIFTandTracker_vs_YOLO_Scenario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kuliah\Tugas Akhir\05111540000055_PBaskara\src\saved_weights\SIFTandTracker_vs_YOLO_Scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,13 +358,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H139" sqref="H139"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="K140" sqref="K140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -384,7 +384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>95</v>
       </c>
@@ -410,7 +410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>96</v>
       </c>
@@ -436,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>97</v>
       </c>
@@ -462,7 +462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>98</v>
       </c>
@@ -488,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99</v>
       </c>
@@ -514,7 +514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>100</v>
       </c>
@@ -540,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>101</v>
       </c>
@@ -566,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>102</v>
       </c>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>103</v>
       </c>
@@ -618,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>104</v>
       </c>
@@ -644,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>105</v>
       </c>
@@ -670,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>106</v>
       </c>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>107</v>
       </c>
@@ -722,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>108</v>
       </c>
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>109</v>
       </c>
@@ -774,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>110</v>
       </c>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>111</v>
       </c>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>112</v>
       </c>
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>113</v>
       </c>
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>114</v>
       </c>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>115</v>
       </c>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>116</v>
       </c>
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>117</v>
       </c>
@@ -982,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>118</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>119</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>120</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>121</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>122</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>123</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>324</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>325</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>326</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>327</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>328</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>329</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>330</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>331</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>332</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>333</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>334</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>335</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>336</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>337</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>338</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>339</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>340</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>341</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>342</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>343</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>344</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>345</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>346</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>347</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>348</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>349</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>69.811320754716974</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>350</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>351</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>452</v>
       </c>
@@ -1854,8 +1854,12 @@
       <c r="D59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <f>(136+53)</f>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>453</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>454</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>455</v>
       </c>
@@ -1897,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>456</v>
       </c>
@@ -1911,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>457</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>458</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>459</v>
       </c>
@@ -1953,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>460</v>
       </c>
@@ -1967,7 +1971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>461</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>462</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>463</v>
       </c>
@@ -2009,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>464</v>
       </c>
@@ -2023,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>465</v>
       </c>
@@ -2037,7 +2041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>466</v>
       </c>
@@ -2051,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>467</v>
       </c>
@@ -2065,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>468</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>469</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>470</v>
       </c>
@@ -2107,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>471</v>
       </c>
@@ -2121,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>472</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>473</v>
       </c>
@@ -2149,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>474</v>
       </c>
@@ -2163,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>475</v>
       </c>
@@ -2177,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>476</v>
       </c>
@@ -2191,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>477</v>
       </c>
@@ -2205,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>478</v>
       </c>
@@ -2219,7 +2223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>479</v>
       </c>
@@ -2233,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>480</v>
       </c>
@@ -2247,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>481</v>
       </c>
@@ -2261,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>482</v>
       </c>
@@ -2275,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>483</v>
       </c>
@@ -2289,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>484</v>
       </c>
@@ -2303,7 +2307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>485</v>
       </c>
@@ -2317,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>486</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>575</v>
       </c>
@@ -2345,7 +2349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>576</v>
       </c>
@@ -2359,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>577</v>
       </c>
@@ -2373,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>578</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>579</v>
       </c>
@@ -2401,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>580</v>
       </c>
@@ -2415,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>581</v>
       </c>
@@ -2429,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>582</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>583</v>
       </c>
@@ -2457,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>584</v>
       </c>
@@ -2471,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>585</v>
       </c>
@@ -2485,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>586</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>587</v>
       </c>
@@ -2513,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>588</v>
       </c>
@@ -2527,7 +2531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>589</v>
       </c>
@@ -2541,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>590</v>
       </c>
@@ -2555,7 +2559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>591</v>
       </c>
@@ -2569,7 +2573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>592</v>
       </c>
@@ -2583,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>593</v>
       </c>
@@ -2597,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>594</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>595</v>
       </c>
@@ -2625,7 +2629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>596</v>
       </c>
@@ -2639,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>597</v>
       </c>
@@ -2653,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>598</v>
       </c>
@@ -2667,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>599</v>
       </c>
@@ -2681,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>600</v>
       </c>
@@ -2695,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>601</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>634</v>
       </c>
@@ -2723,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>635</v>
       </c>
@@ -2737,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>636</v>
       </c>
@@ -2751,7 +2755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>637</v>
       </c>
@@ -2765,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>638</v>
       </c>
@@ -2779,7 +2783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>639</v>
       </c>
@@ -2793,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>640</v>
       </c>
@@ -2807,7 +2811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>641</v>
       </c>
@@ -2821,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>642</v>
       </c>
@@ -2835,7 +2839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>643</v>
       </c>
@@ -2849,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>644</v>
       </c>
@@ -2863,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>645</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>646</v>
       </c>
@@ -2891,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>647</v>
       </c>
@@ -2905,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>648</v>
       </c>
@@ -2919,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>649</v>
       </c>
@@ -2933,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>650</v>
       </c>
@@ -2947,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B138">
         <f>SUM(B2:B137)</f>
         <v>136</v>
@@ -2961,7 +2965,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>1</v>
       </c>

</xml_diff>